<commit_message>
1. Fix RDP utils issue 2. Add flag after all test finished 3. After test finished, check flag.txt, if finished do not send email 4. Modify App Persistent/No Persistent check logic with launch delay 5.Fix get IP and mac exception(os.popen(cmd)) if launch from services
</commit_message>
<xml_diff>
--- a/Test_Suite/citrix_delete.xlsx
+++ b/Test_Suite/citrix_delete.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Z:\WorkSpace3\HPEasyShell\Test_Suite\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F17B9C3-B8FA-4AAA-A481-7751F0316E55}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2865FF26-0A43-4EFA-B7E1-344E499C19A9}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -49,13 +49,13 @@
     <t>EasyshellLib.CommonUtils.Reboot()</t>
   </si>
   <si>
-    <t>Shell_Citrix().utils('standardCitrix', 'Delete')</t>
-  </si>
-  <si>
-    <t>Shell_Citrix().utils('standardCitrix', 'NotExist')</t>
-  </si>
-  <si>
     <t>EasyshellLib.CommonUtils.SwitchToAdmin()</t>
+  </si>
+  <si>
+    <t>Shell_Citrix().utils('standardCitrix', 'Delete', "conn")</t>
+  </si>
+  <si>
+    <t>Shell_Citrix().utils('standardCitrix', 'NotExist', "conn")</t>
   </si>
 </sst>
 </file>
@@ -382,7 +382,7 @@
   <dimension ref="A1:D55"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -422,7 +422,7 @@
         <v>4</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.3">
@@ -446,7 +446,7 @@
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.3">
@@ -454,7 +454,7 @@
         <v>5</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>